<commit_message>
svm ready for run
</commit_message>
<xml_diff>
--- a/Output/Classifier Fitting/SVM/VGG Training Statistics.xlsx
+++ b/Output/Classifier Fitting/SVM/VGG Training Statistics.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>28.92970968484878</v>
+        <v>0.05271441539128621</v>
       </c>
       <c r="C2" t="n">
-        <v>0.004819208676469896</v>
+        <v>0.0008785735898547702</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9431950691321006</v>
+        <v>0.8166666666666667</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8697316125451013</v>
+        <v>0.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>